<commit_message>
BCRA-84 - Update Questionnaire to match final prototype
Change-Id: Ia4b72776f8f6f00835f22e96db5f03a1ef6e71e2
</commit_message>
<xml_diff>
--- a/data/questionnaires/version1/display_condition.xlsx
+++ b/data/questionnaires/version1/display_condition.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>SELF_BREAST_BIOPSY_DIAGNOSIS_RISK_YES</t>
+  </si>
+  <si>
+    <t>FAMILY_BREAST_AFFECTED_MOTHER</t>
+  </si>
+  <si>
+    <t>FAMILY_BREAST_HOW_MANY_ONE</t>
+  </si>
+  <si>
+    <t>FAMILY_OVARIAN_AFFECTED_MOTHER</t>
+  </si>
+  <si>
+    <t>FAMILY_OVARIAN_HOW_MANY_ONE</t>
   </si>
 </sst>
 </file>
@@ -123,10 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -150,6 +159,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -454,34 +468,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" customWidth="1"/>
-    <col min="11" max="11" width="46.140625" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
@@ -491,445 +500,685 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="9">
+      <c r="B2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="23">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E2" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="23">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="B4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="23">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="B5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="23">
         <v>3</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="23">
+        <v>3</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="8">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="23">
+        <v>3</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="8">
-        <v>6</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4">
-        <v>7</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4">
-        <v>7</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
         <v>15</v>
       </c>
-      <c r="D13" s="4">
-        <v>8</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="4">
-        <v>8</v>
+      <c r="C14" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="25">
+        <v>4</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25">
+        <v>4</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="26" t="s">
         <v>9</v>
       </c>
+      <c r="D16" s="25">
+        <v>4</v>
+      </c>
       <c r="E16" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="4">
-        <v>9</v>
+      <c r="C17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="25">
+        <v>4</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="25">
+        <v>4</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="4">
-        <v>10</v>
+      <c r="C19" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="25">
+        <v>4</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="5">
-        <v>10</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4">
-        <v>30</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4">
-        <v>34</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="1">
+        <v>8</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="2">
+        <v>8</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4">
-        <v>36</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F34" s="3"/>
-      <c r="G34" s="1"/>
+      <c r="D40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>